<commit_message>
add agent to conf
add agent to conf
</commit_message>
<xml_diff>
--- a/SensorsSchedulerOutLight_clean.xlsx
+++ b/SensorsSchedulerOutLight_clean.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="9780" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="14355" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GeneralData2" sheetId="13" r:id="rId1"/>
@@ -845,8 +845,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2133,8 +2133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2186,6 +2186,9 @@
       <c r="A3">
         <v>1</v>
       </c>
+      <c r="B3">
+        <v>6</v>
+      </c>
       <c r="D3">
         <v>3</v>
       </c>
@@ -2194,6 +2197,9 @@
       <c r="A4">
         <v>2</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="D4">
         <v>6</v>
       </c>
@@ -2202,6 +2208,9 @@
       <c r="A5">
         <v>3</v>
       </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
       <c r="D5">
         <v>9</v>
       </c>
@@ -2210,6 +2219,9 @@
       <c r="A6">
         <v>4</v>
       </c>
+      <c r="B6">
+        <v>7</v>
+      </c>
       <c r="D6">
         <v>12</v>
       </c>
@@ -2218,6 +2230,9 @@
       <c r="A7">
         <v>5</v>
       </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
       <c r="D7">
         <v>15</v>
       </c>
@@ -2226,6 +2241,9 @@
       <c r="A8">
         <v>6</v>
       </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
       <c r="D8">
         <v>18.25</v>
       </c>
@@ -2233,6 +2251,9 @@
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
       <c r="D9">
         <v>21.25</v>

</xml_diff>